<commit_message>
New approach implemented for FERT
</commit_message>
<xml_diff>
--- a/src/class_CHEM/results_template.xlsx
+++ b/src/class_CHEM/results_template.xlsx
@@ -12,10 +12,6 @@
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -64,7 +60,34 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -399,7 +422,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:Q2"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,22 +468,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1 G1:G1048576 I3:I1048576 M1:M1048576 K1:K1048576">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="11" priority="6">
       <formula>G1&lt;&gt;F1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="10" priority="5">
       <formula>$B1=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="9" priority="4">
       <formula>I2&lt;&gt;H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576 K1:K1048576">
-    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="3" stopIfTrue="1">
       <formula>$C1=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -470,32 +493,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
     <col min="12" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" customWidth="1"/>
-    <col min="14" max="14" width="64.7109375" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" customWidth="1"/>
-    <col min="16" max="16" width="49.140625" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="45.7109375" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="68.42578125" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" customWidth="1"/>
+    <col min="16" max="16" width="56.42578125" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="56.42578125" customWidth="1"/>
+    <col min="19" max="19" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -518,23 +542,23 @@
       <c r="Q1" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I1 G1:G2 M1:M2 K1:K2">
-    <cfRule type="expression" dxfId="3" priority="6">
+  <conditionalFormatting sqref="I1 G1:G1048576 I3:I1048576 M1:M1048576 K1:K1048576">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>G1&lt;&gt;F1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A2">
-    <cfRule type="expression" dxfId="2" priority="5">
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$B1=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>I2&lt;&gt;H2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I2 K1:K2">
-    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="I1:I1048576 K1:K1048576">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>$C1=""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>